<commit_message>
update data va lcn
</commit_message>
<xml_diff>
--- a/file/file.xlsx
+++ b/file/file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>STT</t>
   </si>
@@ -50,7 +50,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>11/12/2023</t>
+    <t>05/12/2023</t>
   </si>
   <si>
     <t>A1</t>
@@ -62,22 +62,22 @@
     <t>Nguyễn Văn An</t>
   </si>
   <si>
-    <t>28.0h</t>
-  </si>
-  <si>
-    <t>210.0</t>
-  </si>
-  <si>
-    <t>59,250,000 VND</t>
-  </si>
-  <si>
-    <t>37,012,500 VND</t>
+    <t>20.0h</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>800,000 VND</t>
+  </si>
+  <si>
+    <t>2,025,000 VND</t>
   </si>
   <si>
     <t>700,000 VND</t>
   </si>
   <si>
-    <t>96,962,500 VND</t>
+    <t>3,525,000 VND</t>
   </si>
   <si>
     <t>2</t>
@@ -92,13 +92,13 @@
     <t>Phạm Thị Bình</t>
   </si>
   <si>
-    <t>53,400,000 VND</t>
-  </si>
-  <si>
-    <t>31,500,000 VND</t>
-  </si>
-  <si>
-    <t>85,600,000 VND</t>
+    <t>1,705,000 VND</t>
+  </si>
+  <si>
+    <t>525,000 VND</t>
+  </si>
+  <si>
+    <t>2,930,000 VND</t>
   </si>
   <si>
     <t>3</t>
@@ -113,19 +113,88 @@
     <t>Vũ Văn Minh</t>
   </si>
   <si>
-    <t>20.0h</t>
-  </si>
-  <si>
-    <t>150.0</t>
-  </si>
-  <si>
-    <t>23,100,000 VND</t>
-  </si>
-  <si>
-    <t>24,750,000 VND</t>
-  </si>
-  <si>
-    <t>48,550,000 VND</t>
+    <t>130.0</t>
+  </si>
+  <si>
+    <t>2,610,000 VND</t>
+  </si>
+  <si>
+    <t>0 VND</t>
+  </si>
+  <si>
+    <t>3,310,000 VND</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>CN0004</t>
+  </si>
+  <si>
+    <t>Trần Thị Mai</t>
+  </si>
+  <si>
+    <t>12.0h</t>
+  </si>
+  <si>
+    <t>1,837,500 VND</t>
+  </si>
+  <si>
+    <t>2,537,500 VND</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>CN0006</t>
+  </si>
+  <si>
+    <t>Hoàng Thị Ngọc</t>
+  </si>
+  <si>
+    <t>1,323,000 VND</t>
+  </si>
+  <si>
+    <t>2,023,000 VND</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>CN0007</t>
+  </si>
+  <si>
+    <t>Phạm Văn Tuấn</t>
+  </si>
+  <si>
+    <t>24.0h</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>1,640,000 VND</t>
+  </si>
+  <si>
+    <t>270,000 VND</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>CN0008</t>
+  </si>
+  <si>
+    <t>Trần Thị Lan</t>
+  </si>
+  <si>
+    <t>1,237,500 VND</t>
+  </si>
+  <si>
+    <t>570,000 VND</t>
+  </si>
+  <si>
+    <t>2,507,500 VND</t>
   </si>
 </sst>
 </file>
@@ -170,7 +239,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -298,22 +367,162 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
         <v>36</v>
       </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>